<commit_message>
Add processing for air extraction of 'Water, CN' from SimaPro exports
</commit_message>
<xml_diff>
--- a/bw2io/data/lci/SimaPro - ecoinvent - biosphere.xlsx
+++ b/bw2io/data/lci/SimaPro - ecoinvent - biosphere.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26819"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23460" windowHeight="26600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="ee" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="787">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1837" uniqueCount="788">
   <si>
     <t>Silver, ion</t>
   </si>
@@ -2385,6 +2385,9 @@
   </si>
   <si>
     <t>Benzene, dichloro-</t>
+  </si>
+  <si>
+    <t>x "Wat</t>
   </si>
 </sst>
 </file>
@@ -2436,8 +2439,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2452,24 +2459,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2737,7 +2740,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2745,11 +2748,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C483"/>
+  <dimension ref="A1:C548"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <pane ySplit="1" topLeftCell="A511" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A552" sqref="A552"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2841,7 +2844,7 @@
         <v>472</v>
       </c>
       <c r="B8" t="s">
-        <v>150</v>
+        <v>787</v>
       </c>
       <c r="C8" t="s">
         <v>234</v>
@@ -8069,6 +8072,721 @@
         <v>752</v>
       </c>
       <c r="C483" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="484" spans="1:3">
+      <c r="A484" t="s">
+        <v>472</v>
+      </c>
+      <c r="B484" t="s">
+        <v>554</v>
+      </c>
+      <c r="C484" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="485" spans="1:3">
+      <c r="A485" t="s">
+        <v>472</v>
+      </c>
+      <c r="B485" t="s">
+        <v>555</v>
+      </c>
+      <c r="C485" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="486" spans="1:3">
+      <c r="A486" t="s">
+        <v>472</v>
+      </c>
+      <c r="B486" t="s">
+        <v>556</v>
+      </c>
+      <c r="C486" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="487" spans="1:3">
+      <c r="A487" t="s">
+        <v>472</v>
+      </c>
+      <c r="B487" t="s">
+        <v>557</v>
+      </c>
+      <c r="C487" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="488" spans="1:3">
+      <c r="A488" t="s">
+        <v>472</v>
+      </c>
+      <c r="B488" t="s">
+        <v>558</v>
+      </c>
+      <c r="C488" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="489" spans="1:3">
+      <c r="A489" t="s">
+        <v>472</v>
+      </c>
+      <c r="B489" t="s">
+        <v>559</v>
+      </c>
+      <c r="C489" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="490" spans="1:3">
+      <c r="A490" t="s">
+        <v>472</v>
+      </c>
+      <c r="B490" t="s">
+        <v>560</v>
+      </c>
+      <c r="C490" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="491" spans="1:3">
+      <c r="A491" t="s">
+        <v>472</v>
+      </c>
+      <c r="B491" t="s">
+        <v>561</v>
+      </c>
+      <c r="C491" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="492" spans="1:3">
+      <c r="A492" t="s">
+        <v>472</v>
+      </c>
+      <c r="B492" t="s">
+        <v>562</v>
+      </c>
+      <c r="C492" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="493" spans="1:3">
+      <c r="A493" t="s">
+        <v>472</v>
+      </c>
+      <c r="B493" t="s">
+        <v>563</v>
+      </c>
+      <c r="C493" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="494" spans="1:3">
+      <c r="A494" t="s">
+        <v>472</v>
+      </c>
+      <c r="B494" t="s">
+        <v>378</v>
+      </c>
+      <c r="C494" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="495" spans="1:3">
+      <c r="A495" t="s">
+        <v>472</v>
+      </c>
+      <c r="B495" t="s">
+        <v>564</v>
+      </c>
+      <c r="C495" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="496" spans="1:3">
+      <c r="A496" t="s">
+        <v>472</v>
+      </c>
+      <c r="B496" t="s">
+        <v>565</v>
+      </c>
+      <c r="C496" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="497" spans="1:3">
+      <c r="A497" t="s">
+        <v>472</v>
+      </c>
+      <c r="B497" t="s">
+        <v>566</v>
+      </c>
+      <c r="C497" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="498" spans="1:3">
+      <c r="A498" t="s">
+        <v>472</v>
+      </c>
+      <c r="B498" t="s">
+        <v>567</v>
+      </c>
+      <c r="C498" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="499" spans="1:3">
+      <c r="A499" t="s">
+        <v>472</v>
+      </c>
+      <c r="B499" t="s">
+        <v>568</v>
+      </c>
+      <c r="C499" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="500" spans="1:3">
+      <c r="A500" t="s">
+        <v>472</v>
+      </c>
+      <c r="B500" t="s">
+        <v>569</v>
+      </c>
+      <c r="C500" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="501" spans="1:3">
+      <c r="A501" t="s">
+        <v>472</v>
+      </c>
+      <c r="B501" t="s">
+        <v>570</v>
+      </c>
+      <c r="C501" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="502" spans="1:3">
+      <c r="A502" t="s">
+        <v>472</v>
+      </c>
+      <c r="B502" t="s">
+        <v>571</v>
+      </c>
+      <c r="C502" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="503" spans="1:3">
+      <c r="A503" t="s">
+        <v>472</v>
+      </c>
+      <c r="B503" t="s">
+        <v>572</v>
+      </c>
+      <c r="C503" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="504" spans="1:3">
+      <c r="A504" t="s">
+        <v>472</v>
+      </c>
+      <c r="B504" t="s">
+        <v>573</v>
+      </c>
+      <c r="C504" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="505" spans="1:3">
+      <c r="A505" t="s">
+        <v>472</v>
+      </c>
+      <c r="B505" t="s">
+        <v>574</v>
+      </c>
+      <c r="C505" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="506" spans="1:3">
+      <c r="A506" t="s">
+        <v>472</v>
+      </c>
+      <c r="B506" t="s">
+        <v>575</v>
+      </c>
+      <c r="C506" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="507" spans="1:3">
+      <c r="A507" t="s">
+        <v>472</v>
+      </c>
+      <c r="B507" t="s">
+        <v>576</v>
+      </c>
+      <c r="C507" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="508" spans="1:3">
+      <c r="A508" t="s">
+        <v>472</v>
+      </c>
+      <c r="B508" t="s">
+        <v>577</v>
+      </c>
+      <c r="C508" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="509" spans="1:3">
+      <c r="A509" t="s">
+        <v>472</v>
+      </c>
+      <c r="B509" t="s">
+        <v>578</v>
+      </c>
+      <c r="C509" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="510" spans="1:3">
+      <c r="A510" t="s">
+        <v>472</v>
+      </c>
+      <c r="B510" t="s">
+        <v>579</v>
+      </c>
+      <c r="C510" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="511" spans="1:3">
+      <c r="A511" t="s">
+        <v>472</v>
+      </c>
+      <c r="B511" t="s">
+        <v>580</v>
+      </c>
+      <c r="C511" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="512" spans="1:3">
+      <c r="A512" t="s">
+        <v>472</v>
+      </c>
+      <c r="B512" t="s">
+        <v>581</v>
+      </c>
+      <c r="C512" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="513" spans="1:3">
+      <c r="A513" t="s">
+        <v>472</v>
+      </c>
+      <c r="B513" t="s">
+        <v>582</v>
+      </c>
+      <c r="C513" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="514" spans="1:3">
+      <c r="A514" t="s">
+        <v>472</v>
+      </c>
+      <c r="B514" t="s">
+        <v>583</v>
+      </c>
+      <c r="C514" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="515" spans="1:3">
+      <c r="A515" t="s">
+        <v>472</v>
+      </c>
+      <c r="B515" t="s">
+        <v>584</v>
+      </c>
+      <c r="C515" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="516" spans="1:3">
+      <c r="A516" t="s">
+        <v>472</v>
+      </c>
+      <c r="B516" t="s">
+        <v>585</v>
+      </c>
+      <c r="C516" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="517" spans="1:3">
+      <c r="A517" t="s">
+        <v>472</v>
+      </c>
+      <c r="B517" t="s">
+        <v>586</v>
+      </c>
+      <c r="C517" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="518" spans="1:3">
+      <c r="A518" t="s">
+        <v>472</v>
+      </c>
+      <c r="B518" t="s">
+        <v>587</v>
+      </c>
+      <c r="C518" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="519" spans="1:3">
+      <c r="A519" t="s">
+        <v>472</v>
+      </c>
+      <c r="B519" t="s">
+        <v>588</v>
+      </c>
+      <c r="C519" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="520" spans="1:3">
+      <c r="A520" t="s">
+        <v>472</v>
+      </c>
+      <c r="B520" t="s">
+        <v>589</v>
+      </c>
+      <c r="C520" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="521" spans="1:3">
+      <c r="A521" t="s">
+        <v>472</v>
+      </c>
+      <c r="B521" t="s">
+        <v>590</v>
+      </c>
+      <c r="C521" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="522" spans="1:3">
+      <c r="A522" t="s">
+        <v>472</v>
+      </c>
+      <c r="B522" t="s">
+        <v>591</v>
+      </c>
+      <c r="C522" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="523" spans="1:3">
+      <c r="A523" t="s">
+        <v>472</v>
+      </c>
+      <c r="B523" t="s">
+        <v>592</v>
+      </c>
+      <c r="C523" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="524" spans="1:3">
+      <c r="A524" t="s">
+        <v>472</v>
+      </c>
+      <c r="B524" t="s">
+        <v>593</v>
+      </c>
+      <c r="C524" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="525" spans="1:3">
+      <c r="A525" t="s">
+        <v>472</v>
+      </c>
+      <c r="B525" t="s">
+        <v>594</v>
+      </c>
+      <c r="C525" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="526" spans="1:3">
+      <c r="A526" t="s">
+        <v>472</v>
+      </c>
+      <c r="B526" t="s">
+        <v>595</v>
+      </c>
+      <c r="C526" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="527" spans="1:3">
+      <c r="A527" t="s">
+        <v>472</v>
+      </c>
+      <c r="B527" t="s">
+        <v>596</v>
+      </c>
+      <c r="C527" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="528" spans="1:3">
+      <c r="A528" t="s">
+        <v>472</v>
+      </c>
+      <c r="B528" t="s">
+        <v>597</v>
+      </c>
+      <c r="C528" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="529" spans="1:3">
+      <c r="A529" t="s">
+        <v>472</v>
+      </c>
+      <c r="B529" t="s">
+        <v>598</v>
+      </c>
+      <c r="C529" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="530" spans="1:3">
+      <c r="A530" t="s">
+        <v>472</v>
+      </c>
+      <c r="B530" t="s">
+        <v>599</v>
+      </c>
+      <c r="C530" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="531" spans="1:3">
+      <c r="A531" t="s">
+        <v>472</v>
+      </c>
+      <c r="B531" t="s">
+        <v>600</v>
+      </c>
+      <c r="C531" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="532" spans="1:3">
+      <c r="A532" t="s">
+        <v>472</v>
+      </c>
+      <c r="B532" t="s">
+        <v>601</v>
+      </c>
+      <c r="C532" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="533" spans="1:3">
+      <c r="A533" t="s">
+        <v>472</v>
+      </c>
+      <c r="B533" t="s">
+        <v>602</v>
+      </c>
+      <c r="C533" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="534" spans="1:3">
+      <c r="A534" t="s">
+        <v>472</v>
+      </c>
+      <c r="B534" t="s">
+        <v>603</v>
+      </c>
+      <c r="C534" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="535" spans="1:3">
+      <c r="A535" t="s">
+        <v>472</v>
+      </c>
+      <c r="B535" t="s">
+        <v>604</v>
+      </c>
+      <c r="C535" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="536" spans="1:3">
+      <c r="A536" t="s">
+        <v>472</v>
+      </c>
+      <c r="B536" t="s">
+        <v>605</v>
+      </c>
+      <c r="C536" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="537" spans="1:3">
+      <c r="A537" t="s">
+        <v>472</v>
+      </c>
+      <c r="B537" t="s">
+        <v>606</v>
+      </c>
+      <c r="C537" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="538" spans="1:3">
+      <c r="A538" t="s">
+        <v>472</v>
+      </c>
+      <c r="B538" t="s">
+        <v>607</v>
+      </c>
+      <c r="C538" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="539" spans="1:3">
+      <c r="A539" t="s">
+        <v>472</v>
+      </c>
+      <c r="B539" t="s">
+        <v>608</v>
+      </c>
+      <c r="C539" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="540" spans="1:3">
+      <c r="A540" t="s">
+        <v>472</v>
+      </c>
+      <c r="B540" t="s">
+        <v>609</v>
+      </c>
+      <c r="C540" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="541" spans="1:3">
+      <c r="A541" t="s">
+        <v>472</v>
+      </c>
+      <c r="B541" t="s">
+        <v>610</v>
+      </c>
+      <c r="C541" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="542" spans="1:3">
+      <c r="A542" t="s">
+        <v>472</v>
+      </c>
+      <c r="B542" t="s">
+        <v>611</v>
+      </c>
+      <c r="C542" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="543" spans="1:3">
+      <c r="A543" t="s">
+        <v>472</v>
+      </c>
+      <c r="B543" t="s">
+        <v>612</v>
+      </c>
+      <c r="C543" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="544" spans="1:3">
+      <c r="A544" t="s">
+        <v>472</v>
+      </c>
+      <c r="B544" t="s">
+        <v>613</v>
+      </c>
+      <c r="C544" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="545" spans="1:3">
+      <c r="A545" t="s">
+        <v>472</v>
+      </c>
+      <c r="B545" t="s">
+        <v>614</v>
+      </c>
+      <c r="C545" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="546" spans="1:3">
+      <c r="A546" t="s">
+        <v>472</v>
+      </c>
+      <c r="B546" t="s">
+        <v>615</v>
+      </c>
+      <c r="C546" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="547" spans="1:3">
+      <c r="A547" t="s">
+        <v>472</v>
+      </c>
+      <c r="B547" t="s">
+        <v>616</v>
+      </c>
+      <c r="C547" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="548" spans="1:3">
+      <c r="A548" t="s">
+        <v>472</v>
+      </c>
+      <c r="B548" t="s">
+        <v>617</v>
+      </c>
+      <c r="C548" t="s">
         <v>490</v>
       </c>
     </row>

</xml_diff>